<commit_message>
cal efficient frontier ok
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookp/Desktop/Duke/Semester2023spring/fintech512/GroupProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C180A-A4C3-7A49-94BE-42340A89AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97011F90-BFA0-D04A-B271-11DA4853F9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="10400" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:H1250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>